<commit_message>
fix apar report checksheet
</commit_message>
<xml_diff>
--- a/public/templates/template-checksheet-powder.xlsx
+++ b/public/templates/template-checksheet-powder.xlsx
@@ -1,35 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
-  <x:workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\03_Maintenance\Safety &amp; Environment\01. SAFETY\Checksheet &amp; Form\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00_DATA\itd.magang01\Desktop\Apar\Check Sheet\Check Sheet Satuan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C735EF1-FC31-4817-895A-7A1CA37E240D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="POWDER" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="_xlnm.Print_Area" localSheetId="1">'CO2'!$A$1:$AO$28</x:definedName>
-    <x:definedName name="_xlnm.Print_Area" localSheetId="0">POWDER!$A$1:$AR$25</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="152511"/>
-  <x:extLst>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51904AAF-1889-4142-8ED5-92401FCF53F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="POWDER" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">POWDER!$A$1:$AR$25</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>PT. AISIN INDONESIA AUTOMOTIVE</t>
   </si>
@@ -90,12 +89,6 @@
     <t xml:space="preserve">    DILAKUKAN DENGAN CARA DI BOLAK-BALIKAN TABUNG 3-4 KALI </t>
   </si>
   <si>
-    <t>BERAT TABUNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - UNTUK APAR TIPE CO2 METODE PENGECEKAN BERAT TABUNGNYA</t>
-  </si>
-  <si>
     <t>KADAR KONSENTRAT (POWDER)</t>
   </si>
   <si>
@@ -105,12 +98,6 @@
     <t>SERBUK JATUH JIKA NG SUARA SEPERTI BENTURAN</t>
   </si>
   <si>
-    <t xml:space="preserve">    DILAKUKAN DENGAN CARA DI TIMBANG JIKA BERAT BERKURANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    10 % MAKA APAR DINYATAKAN NG</t>
-  </si>
-  <si>
     <t>TABUNG</t>
   </si>
   <si>
@@ -123,10 +110,7 @@
     <t xml:space="preserve">   SERBUK JATUH. JIKA NG SUARA SEPERTI BENTURAN </t>
   </si>
   <si>
-    <t>CORONG / NOZZLE</t>
-  </si>
-  <si>
-    <t>TAHUN: 2022</t>
+    <t xml:space="preserve">TAHUN: </t>
   </si>
 </sst>
 </file>
@@ -205,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,18 +198,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -452,86 +430,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -604,13 +507,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,63 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,8 +934,8 @@
   </sheetPr>
   <dimension ref="B1:AR25"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="AZ11" sqref="AZ11"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="BC9" sqref="BC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,7 +1195,7 @@
       <c r="P6" s="21"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="S6" s="18"/>
       <c r="T6" s="18"/>
@@ -1373,7 +1219,7 @@
       <c r="AK6" s="21"/>
       <c r="AL6" s="22"/>
       <c r="AM6" s="17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="AN6" s="18"/>
       <c r="AO6" s="18"/>
@@ -1511,12 +1357,12 @@
       </c>
       <c r="M9" s="40"/>
       <c r="N9" s="41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O9" s="45"/>
       <c r="P9" s="42"/>
       <c r="Q9" s="40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R9" s="40"/>
       <c r="S9" s="40"/>
@@ -1544,11 +1390,11 @@
       </c>
       <c r="AI9" s="40"/>
       <c r="AJ9" s="41" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AK9" s="42"/>
       <c r="AL9" s="40" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AM9" s="40"/>
       <c r="AN9" s="40"/>
@@ -2098,12 +1944,12 @@
     <row r="23" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="F23" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W23" s="5"/>
       <c r="Y23" s="4"/>
       <c r="AC23" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AR23" s="5"/>
     </row>
@@ -2113,12 +1959,12 @@
         <v>15</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="W24" s="5"/>
       <c r="Y24" s="4"/>
       <c r="AC24" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AR24" s="5"/>
     </row>
@@ -2128,7 +1974,7 @@
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -2152,7 +1998,7 @@
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
       <c r="AC25" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AD25" s="7"/>
       <c r="AE25" s="7"/>

</xml_diff>